<commit_message>
Update Excel data and optimize downloader (10 workers)
</commit_message>
<xml_diff>
--- a/data/BAF.xlsx
+++ b/data/BAF.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="336">
   <si>
     <t>Liên Hệ</t>
   </si>
@@ -73,7 +73,7 @@
     <t>Ngày xuất</t>
   </si>
   <si>
-    <t>26/11/2025</t>
+    <t>17/12/2025</t>
   </si>
   <si>
     <t>BAF</t>
@@ -13414,7 +13414,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF32B87-0276-EF4E-963C-ED48B34C3BF9}">
-  <dimension ref="A1:Y60"/>
+  <dimension ref="A1:Z60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -13447,6 +13447,7 @@
     <col min="23" max="23" width="17.453125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.5390625" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="19.19921875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="18.5390625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13565,6 +13566,9 @@
       <c r="Y11" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="Z11" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="24" t="s">
@@ -13639,6 +13643,9 @@
       <c r="Y12" s="21" t="n">
         <v>2.12300591806E11</v>
       </c>
+      <c r="Z12" s="21" t="n">
+        <v>2.6425997639E10</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="24" t="s">
@@ -13713,6 +13720,9 @@
       <c r="Y13" s="21" t="n">
         <v>6.0068787542E10</v>
       </c>
+      <c r="Z13" s="21" t="n">
+        <v>6.1391145892E10</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="24" t="s">
@@ -13787,6 +13797,9 @@
       <c r="Y14" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="Z14" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="24" t="s">
@@ -13861,6 +13874,9 @@
       <c r="Y15" s="21" t="n">
         <v>2.627406919E9</v>
       </c>
+      <c r="Z15" s="21" t="n">
+        <v>-1.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="24" t="s">
@@ -13935,6 +13951,9 @@
       <c r="Y16" s="21" t="n">
         <v>9.761381E7</v>
       </c>
+      <c r="Z16" s="21" t="n">
+        <v>-2.35473881E8</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="24" t="s">
@@ -14009,6 +14028,9 @@
       <c r="Y17" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="Z17" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="24" t="s">
@@ -14083,6 +14105,9 @@
       <c r="Y18" s="21" t="n">
         <v>-7.002227159E9</v>
       </c>
+      <c r="Z18" s="21" t="n">
+        <v>-4.466214678E9</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="24" t="s">
@@ -14157,6 +14182,9 @@
       <c r="Y19" s="21" t="n">
         <v>6.6218039301E10</v>
       </c>
+      <c r="Z19" s="21" t="n">
+        <v>5.9544362622E10</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="24" t="s">
@@ -14231,6 +14259,9 @@
       <c r="Y20" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="Z20" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="24" t="s">
@@ -14305,6 +14336,9 @@
       <c r="Y21" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="Z21" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="24" t="s">
@@ -14379,6 +14413,9 @@
       <c r="Y22" s="21" t="n">
         <v>-1.510495686056E12</v>
       </c>
+      <c r="Z22" s="21" t="n">
+        <v>8.4910858533E10</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="22" t="s">
@@ -14453,6 +14490,9 @@
       <c r="Y23" s="21" t="n">
         <v>3.34310212219E11</v>
       </c>
+      <c r="Z23" s="21" t="n">
+        <v>1.42659817593E11</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="22" t="s">
@@ -14527,6 +14567,9 @@
       <c r="Y24" s="21" t="n">
         <v>3.05883464944E11</v>
       </c>
+      <c r="Z24" s="21" t="n">
+        <v>-3.85249734842E11</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="22" t="s">
@@ -14601,6 +14644,9 @@
       <c r="Y25" s="21" t="n">
         <v>2.907120594E9</v>
       </c>
+      <c r="Z25" s="21" t="n">
+        <v>-2.76827500901E11</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="22" t="s">
@@ -14675,6 +14721,9 @@
       <c r="Y26" s="21" t="n">
         <v>-2.022672308207E12</v>
       </c>
+      <c r="Z26" s="21" t="n">
+        <v>9.18689175669E11</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="22" t="s">
@@ -14749,6 +14798,9 @@
       <c r="Y27" s="21" t="n">
         <v>-9.9203488182E10</v>
       </c>
+      <c r="Z27" s="21" t="n">
+        <v>-2.35124926932E11</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="22" t="s">
@@ -14823,6 +14875,9 @@
       <c r="Y28" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="Z28" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="22" t="s">
@@ -14897,6 +14952,9 @@
       <c r="Y29" s="21" t="n">
         <v>-3.1857623931E10</v>
       </c>
+      <c r="Z29" s="21" t="n">
+        <v>-7.9235972054E10</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="22" t="s">
@@ -14971,6 +15029,9 @@
       <c r="Y30" s="21" t="n">
         <v>1.36936507E8</v>
       </c>
+      <c r="Z30" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="22" t="s">
@@ -15045,6 +15106,9 @@
       <c r="Y31" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="Z31" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="22" t="s">
@@ -15119,6 +15183,9 @@
       <c r="Y32" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="Z32" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="24" t="s">
@@ -15193,6 +15260,9 @@
       <c r="Y33" s="21" t="n">
         <v>-2.83052029473E11</v>
       </c>
+      <c r="Z33" s="21" t="n">
+        <v>-7.47878034479E11</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="22" t="s">
@@ -15267,6 +15337,9 @@
       <c r="Y34" s="21" t="n">
         <v>-1.89637273103E11</v>
       </c>
+      <c r="Z34" s="21" t="n">
+        <v>-6.45511029583E11</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="22" t="s">
@@ -15341,6 +15414,9 @@
       <c r="Y35" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="Z35" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="22" t="s">
@@ -15415,6 +15491,9 @@
       <c r="Y36" s="21" t="n">
         <v>-3.369312403E9</v>
       </c>
+      <c r="Z36" s="21" t="n">
+        <v>-1.38953812134E11</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="22" t="s">
@@ -15489,6 +15568,9 @@
       <c r="Y37" s="21" t="n">
         <v>7.38737E10</v>
       </c>
+      <c r="Z37" s="21" t="n">
+        <v>-4.8708424537E10</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="22" t="s">
@@ -15563,6 +15645,9 @@
       <c r="Y38" s="21" t="n">
         <v>-1.71558752495E11</v>
       </c>
+      <c r="Z38" s="21" t="n">
+        <v>7.9296164495E10</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="22" t="s">
@@ -15637,6 +15722,9 @@
       <c r="Y39" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="Z39" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="22" t="s">
@@ -15711,6 +15799,9 @@
       <c r="Y40" s="21" t="n">
         <v>7.639608528E9</v>
       </c>
+      <c r="Z40" s="21" t="n">
+        <v>5.99906728E9</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="24" t="s">
@@ -15785,6 +15876,9 @@
       <c r="Y41" s="21" t="n">
         <v>1.351531535944E12</v>
       </c>
+      <c r="Z41" s="21" t="n">
+        <v>4.22783038123E11</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="22" t="s">
@@ -15859,6 +15953,9 @@
       <c r="Y42" s="21" t="n">
         <v>1.00662E12</v>
       </c>
+      <c r="Z42" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="22" t="s">
@@ -15933,6 +16030,9 @@
       <c r="Y43" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="Z43" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="22" t="s">
@@ -16007,6 +16107,9 @@
       <c r="Y44" s="21" t="n">
         <v>9.91693828119E11</v>
       </c>
+      <c r="Z44" s="21" t="n">
+        <v>1.083594753956E12</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="22" t="s">
@@ -16081,6 +16184,9 @@
       <c r="Y45" s="21" t="n">
         <v>-6.44134871451E11</v>
       </c>
+      <c r="Z45" s="21" t="n">
+        <v>-6.57325488575E11</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="22" t="s">
@@ -16155,6 +16261,9 @@
       <c r="Y46" s="21" t="n">
         <v>-2.647420724E9</v>
       </c>
+      <c r="Z46" s="21" t="n">
+        <v>-3.486227258E9</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="22" t="s">
@@ -16229,6 +16338,9 @@
       <c r="Y47" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="Z47" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="22" t="s">
@@ -16303,6 +16415,9 @@
       <c r="Y48" s="21" t="n">
         <v>0.0</v>
       </c>
+      <c r="Z48" s="21" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="24" t="s">
@@ -16377,6 +16492,9 @@
       <c r="Y49" s="21" t="n">
         <v>-4.42016179585E11</v>
       </c>
+      <c r="Z49" s="21" t="n">
+        <v>-2.40184137823E11</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="24" t="s">
@@ -16451,6 +16569,9 @@
       <c r="Y50" s="21" t="n">
         <v>8.24974095909E11</v>
       </c>
+      <c r="Z50" s="21" t="n">
+        <v>3.82959718423E11</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="24" t="s">
@@ -16525,6 +16646,9 @@
       <c r="Y51" s="21" t="n">
         <v>1802099.0</v>
       </c>
+      <c r="Z51" s="21" t="n">
+        <v>713076.0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="24" t="s">
@@ -16599,6 +16723,9 @@
       <c r="Y52" s="21" t="n">
         <v>3.82959718423E11</v>
       </c>
+      <c r="Z52" s="21" t="n">
+        <v>1.42776293676E11</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
@@ -16638,7 +16765,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B10:F10"/>
-    <mergeCell ref="H10:Y10"/>
+    <mergeCell ref="H10:Z10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A58" r:id="rId1" display="https://www.vietcap.com.vn/" xr:uid="{2404128C-51EF-8E44-9BE0-4A8D207DD5D8}"/>

</xml_diff>